<commit_message>
cambios y busqeda general
</commit_message>
<xml_diff>
--- a/SoleraWeb/build/web/WEB-INF/classes/CARGA SOLERA.xlsx
+++ b/SoleraWeb/build/web/WEB-INF/classes/CARGA SOLERA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEAS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\death\Desktop\Solera Web 2\SoleraWeb2\SoleraWeb\src\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E448FA-B067-4124-89F7-EE039B23DACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA493F-7382-4FCD-941A-7D18AD33D9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -2703,9 +2703,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
cabmios a las busqyuedas
</commit_message>
<xml_diff>
--- a/SoleraWeb/build/web/WEB-INF/classes/CARGA SOLERA.xlsx
+++ b/SoleraWeb/build/web/WEB-INF/classes/CARGA SOLERA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\death\Desktop\Solera Web 2\SoleraWeb2\SoleraWeb\src\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEAS\Desktop\SoleraWeb\SoleraWeb\src\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA493F-7382-4FCD-941A-7D18AD33D9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F885800-0184-47E2-B848-C3E7BE6F0D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -2700,10 +2700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A153"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2792,7 +2793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>42147405</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>42172278</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>42118536</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>42129149</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>42152626</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>52</v>
       </c>
@@ -3163,7 +3164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>42164643</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>61</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>72</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>42187629</v>
       </c>
@@ -3428,7 +3429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>80</v>
       </c>
@@ -3481,7 +3482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>42290076</v>
       </c>
@@ -3640,7 +3641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>98</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -3746,7 +3747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>42290090</v>
       </c>
@@ -3799,7 +3800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>110</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>114</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>42219888</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>127</v>
       </c>
@@ -4064,7 +4065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>131</v>
       </c>
@@ -4276,7 +4277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>42220909</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>153</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>158</v>
       </c>
@@ -4435,7 +4436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>163</v>
       </c>
@@ -4488,7 +4489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>168</v>
       </c>
@@ -4541,7 +4542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>172</v>
       </c>
@@ -4647,7 +4648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>42238835</v>
       </c>
@@ -4806,7 +4807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>42247976</v>
       </c>
@@ -4965,7 +4966,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>204</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>211</v>
       </c>
@@ -5124,7 +5125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>215</v>
       </c>
@@ -5177,7 +5178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>218</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>42253434</v>
       </c>
@@ -5601,7 +5602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>253</v>
       </c>
@@ -5654,7 +5655,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>256</v>
       </c>
@@ -5760,7 +5761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>265</v>
       </c>
@@ -5919,7 +5920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>42223774</v>
       </c>
@@ -6025,7 +6026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>42256179</v>
       </c>
@@ -6237,7 +6238,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>42203432</v>
       </c>
@@ -6608,7 +6609,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>42209886</v>
       </c>
@@ -6661,7 +6662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>42235325</v>
       </c>
@@ -6714,7 +6715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>42249655</v>
       </c>
@@ -6820,7 +6821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>42252022</v>
       </c>
@@ -6873,7 +6874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>42252106</v>
       </c>
@@ -6926,7 +6927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>42271411</v>
       </c>
@@ -7138,7 +7139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>346</v>
       </c>
@@ -7403,7 +7404,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>366</v>
       </c>
@@ -7456,7 +7457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>369</v>
       </c>
@@ -7509,7 +7510,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>374</v>
       </c>
@@ -7562,7 +7563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>42235739</v>
       </c>
@@ -7615,7 +7616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>42280136</v>
       </c>
@@ -7668,7 +7669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>42258694</v>
       </c>
@@ -8092,7 +8093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>414</v>
       </c>
@@ -8198,7 +8199,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>42275385</v>
       </c>
@@ -8251,7 +8252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>42215868</v>
       </c>
@@ -8304,7 +8305,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>42271609</v>
       </c>
@@ -8410,7 +8411,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>42253152</v>
       </c>
@@ -8516,7 +8517,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>42271388</v>
       </c>
@@ -8569,7 +8570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>445</v>
       </c>
@@ -8622,7 +8623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
         <v>448</v>
       </c>
@@ -8675,7 +8676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
         <v>452</v>
       </c>
@@ -8781,7 +8782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>42160898</v>
       </c>
@@ -8940,7 +8941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>42208866</v>
       </c>
@@ -8993,7 +8994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>42147035</v>
       </c>
@@ -9046,7 +9047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>42219498</v>
       </c>
@@ -9205,7 +9206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>42264110</v>
       </c>
@@ -9364,7 +9365,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>42238508</v>
       </c>
@@ -9417,7 +9418,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>495</v>
       </c>
@@ -9470,7 +9471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>42159905</v>
       </c>
@@ -9629,7 +9630,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>42120328</v>
       </c>
@@ -9682,7 +9683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>42151241</v>
       </c>
@@ -9735,7 +9736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>513</v>
       </c>
@@ -9788,7 +9789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>42164126</v>
       </c>
@@ -9841,7 +9842,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>42188233</v>
       </c>
@@ -9894,7 +9895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>42227174</v>
       </c>
@@ -9947,7 +9948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>42234951</v>
       </c>
@@ -10106,7 +10107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>534</v>
       </c>
@@ -10159,7 +10160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>42288344</v>
       </c>
@@ -10212,7 +10213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>42271794</v>
       </c>
@@ -10265,7 +10266,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>42260510</v>
       </c>
@@ -10318,7 +10319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>42278304</v>
       </c>
@@ -10371,7 +10372,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>42269552</v>
       </c>
@@ -10424,7 +10425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>42230078</v>
       </c>
@@ -10477,7 +10478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>42242925</v>
       </c>
@@ -10530,7 +10531,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>42162836</v>
       </c>
@@ -10583,7 +10584,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>42287925</v>
       </c>
@@ -10689,7 +10690,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>42265435</v>
       </c>
@@ -10795,7 +10796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>42269653</v>
       </c>
@@ -10849,70 +10850,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q153" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="123LEASE SAPI DE CV//FLORISEL REYES CRUZ"/>
-        <filter val="ABRAHAM RAFAEL SUAREZ HEREDIA//MUNICIPIO DE HIDALGO MICHOACAN"/>
-        <filter val="AGROS HORTICULTORES S.A. DE C.V.//JESUS AVIÑA"/>
-        <filter val="ALD AUTOMOTIVE SA DE CV//JOSE ALBERTO VAZQUEZ RAMIREZ"/>
-        <filter val="ALD AUTOMOTIVE SA DE CV//JOSE ANTONIO GARCIA DIAS"/>
-        <filter val="ALD AUTOMOTIVE SA DE CV//NOHEMI PLANCARTE PULIDO"/>
-        <filter val="ARTURO PEREZ LUNA//FELIPE DE JESUS LOPEZ LEOS"/>
-        <filter val="CARNES SELECTAS ICEA SA DE CV//GUILLERMO ARANDAS PINTO"/>
-        <filter val="CARNES SELECTAS ICEA SA DE CV//MOISES CORDERO INDA"/>
-        <filter val="CARZA ARRENDAMIENTO S.A. DE C.V.//JUAN LUIS HERNANDEZ"/>
-        <filter val="CARZA ARRENDAMIENTO S.A. DE C.V.//SAUL JUAREZ LOPEZ"/>
-        <filter val="COMERCIALIZADORA PUNTO GDL SA DE CV//JOSE EDUARDO ROMERO ALVAREZ"/>
-        <filter val="CORPORATIVO DE PROTECCION SEGURIDAD PRIVADA Y SERV ESPECIALIZADOS SA DE CV//LUIS ANDRES DUARTE PEÃUELAS"/>
-        <filter val="D CONCREFOCC SA DE CV//RAUL ROMERO ARELLANO"/>
-        <filter val="DIMA RODRIGUEZ OVIEDO//MARCELA GUADALUPE IBARRA LOPEZ"/>
-        <filter val="EDGAR RICARDO MONTERO ESPARZA//MUNICIPIO DE TEQUILA JAL"/>
-        <filter val="EDREI HERNÃNDEZ LUGO//ERICK TOSER NUÃO JIMÃNEZ"/>
-        <filter val="ERIC HERNANDEZ DE LA CRUZ   // SAUL BENJAMIN GONZALEZ"/>
-        <filter val="GERARDO HERNANDEZ CAMPOS //MARIA RAMIREZ"/>
-        <filter val="GIRECO SA DE CV//KARINA MERCADO MUNGARAY"/>
-        <filter val="GRUPO INTERMOVIL KREMPDOR S DE RL DE CV//JOSEU CORDOBA NUÃEZ"/>
-        <filter val="GRUPO TRACTOCAMIONES Y AUTOBUSES DEL BAJIO SA DE CV//JORGE DANIEL MARTINEZ"/>
-        <filter val="HELM DE MEXICO SA//GUSTAVO IGNACIO LEMUS MENDIOLA"/>
-        <filter val="INTERNATIONAL BUSINESS AND BEST MONEY SA DE CV//ANTONIO HERNANDEZ"/>
-        <filter val="ISRAEL GONZALEZ RAMIREZ//JUAN CAMARENA"/>
-        <filter val="ISRAEL LOPEZ LOPEZ//ERNESTO DE JESUS MORENO GUTIERREZ"/>
-        <filter val="LEASEPLAN MEXICO SA DE CV//AGUSTIN BLANCO CERVANTES"/>
-        <filter val="LEASEPLAN MEXICO SA DE CV//BRAULIO ALEXIS MALDONADO AGUILAR"/>
-        <filter val="LEASEPLAN MEXICO SA DE CV//EDGAR BARAJAS SEVILLA"/>
-        <filter val="MAGNOCENTRO FERRETERO SA DE CV//RAFAEL MALDONADO MORA"/>
-        <filter val="MANZAHNOS VIAJES SA DE CV//FERNANDO BERNAL//OSCAR MANZANO"/>
-        <filter val="MILAGROS CORONA VERGARA//DANIEL SEGOVIANO SCHMIDT"/>
-        <filter val="MUEBLERIA HIDALGO DEL NOROESTE SA DE CV//JUAN SERRANO"/>
-        <filter val="MUNICIPIO DE LA HUERTA JALISCO//SALVADOR LOPEZ PRECIADO"/>
-        <filter val="MUNICIPIO DE SAN LUIS RIO COLORADO SONORA//GILBERTO ROBLES ZEPEDA"/>
-        <filter val="MUNICIPIO DE SAN PEDRO TLAQUEPAQUE//ÃSCAR FLAVIO PÃREZ ELVIRA"/>
-        <filter val="MUNICIPIO DE SAN PEDRO TLAQUEPAQUE//CARLOS EDUARDO BLADIMIR MURILLO"/>
-        <filter val="MUNICIPIO DE TALA//JOSÃ MANUEL RUIZ QUEZADA"/>
-        <filter val="MUNICIPIO DE TAMAZULA DE GORDIANO JALISCO//CESAR ARMANDO ESQUIVEL TORRES"/>
-        <filter val="MUNICIPIO DE TECOLOTLAN JALISCO//RIGOBERTO ANDRADE RODRIGUEZ"/>
-        <filter val="PIZZA Y COME S.A DE C.V//ROBERTO JAUREGUI LEE"/>
-        <filter val="PRISMA ENVASE SA DE CV//ERNESTO GOMEZ//LENIA RIVERON"/>
-        <filter val="PRO TECH INTERNATIONAL SERVICES S.A. DE C.V.//ALFREDO OLIVARES FERNANDEZ"/>
-        <filter val="RAFAEL GARCIA VAES//MA ESTELA BAEZ ALVAREZ"/>
-        <filter val="RICARDO PEñA//ANA IRENE GUADALUPE BARAJAS MARTINEZ"/>
-        <filter val="RUBEN HEREDIA LARIOS//GABRIEL HEREDIA TORRES"/>
-        <filter val="SANCHEZ SA DE CV//HECTOR ARIAS MORENO"/>
-        <filter val="SEMIRE SA DE CV//MISAEL OCHOA MENDEZ"/>
-        <filter val="SERVICIOS INTEGRALES EN EL MANEJO DEL AMBIENTE S DE RL DE CV// LETICIA JIMENEZ ESQUIVEL"/>
-        <filter val="SOCIEDAD ECOLOGICA PARA EL MANEJO DE RESIDUOS SA//EDGAR FELIPE NUñO"/>
-        <filter val="SOLUCIONES Y APLICACIONES EN PROCEDIMIENTOS INTRAMUROS SA DE CV//FREDY MAGDALENO ZEA"/>
-        <filter val="START BANREGIO SA DE CV SOFOM ER BANREGIO GRUPO FINANCIERO//JUAN MANUEL VEGA FLORES"/>
-        <filter val="SUSPENSION Y DIRECCION SA DE CV//MOISES VAZQUEZ VELASQUEZ"/>
-        <filter val="TACTICA Y TECNOLOGIA EN SEGURIDAD PRIVADA SA DE CV//JAVIER HERNANDEZ// RAFAEL ALTAMIRANO"/>
-        <filter val="TACTICA Y TECNOLOGIA EN SEGURIDAD PRIVADA SA DE CV//ROMULO VILLALOBOS FERNANDEZ"/>
-        <filter val="TRECE CAR RENTAL GROUP SA DE CV//ROBERTO MEDRANO"/>
-        <filter val="UBER PORTIER MEXICO S DE RL DE//SERGIO ANTONIO GOMEZ SAUCEDA"/>
-        <filter val="WIRELESS MOBILE SA DE CV//ABRAHAM MACHADO SANTIAGO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q153" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
carga de comentarios y tabla
</commit_message>
<xml_diff>
--- a/SoleraWeb/build/web/WEB-INF/classes/CARGA SOLERA.xlsx
+++ b/SoleraWeb/build/web/WEB-INF/classes/CARGA SOLERA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEAS\Desktop\SoleraWeb\SoleraWeb\src\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024ABFBE-5A34-4629-A304-7F85839DA163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB91F7A-AB5E-4DF7-911F-975E7D4B6151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2176,7 +2176,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2789,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H67" workbookViewId="0">
-      <selection activeCell="L157" sqref="L157"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3252,7 +3252,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="10">
         <v>42164643</v>
       </c>
       <c r="B9" s="4">
@@ -3305,7 +3305,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="4">
@@ -3358,7 +3358,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="4">
@@ -3411,7 +3411,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="4">
@@ -3464,7 +3464,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="10">
         <v>42187629</v>
       </c>
       <c r="B13" s="4">
@@ -3517,7 +3517,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B14" s="4">
@@ -3570,7 +3570,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="4">
@@ -3623,7 +3623,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="4">
@@ -3676,7 +3676,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="10">
         <v>42290076</v>
       </c>
       <c r="B17" s="4">
@@ -3729,7 +3729,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B18" s="4">
@@ -3782,7 +3782,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B19" s="4">
@@ -3835,7 +3835,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="10">
         <v>42290090</v>
       </c>
       <c r="B20" s="4">
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="10" t="s">
         <v>110</v>
       </c>
       <c r="B21" s="4">
@@ -3941,7 +3941,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="10" t="s">
         <v>114</v>
       </c>
       <c r="B22" s="4">
@@ -3994,7 +3994,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="10">
         <v>42219888</v>
       </c>
       <c r="B23" s="4">
@@ -4047,7 +4047,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="10">
         <v>42137312</v>
       </c>
       <c r="B24" s="4">
@@ -4100,7 +4100,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="10" t="s">
         <v>127</v>
       </c>
       <c r="B25" s="4">
@@ -4153,7 +4153,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="10" t="s">
         <v>131</v>
       </c>
       <c r="B26" s="4">
@@ -4259,7 +4259,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="10" t="s">
         <v>140</v>
       </c>
       <c r="B28" s="4">
@@ -4312,7 +4312,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="10">
         <v>42229972</v>
       </c>
       <c r="B29" s="4">
@@ -4365,7 +4365,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="10">
         <v>42220909</v>
       </c>
       <c r="B30" s="4">
@@ -4418,7 +4418,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="10" t="s">
         <v>153</v>
       </c>
       <c r="B31" s="4">
@@ -4471,7 +4471,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="10" t="s">
         <v>158</v>
       </c>
       <c r="B32" s="4">
@@ -4524,7 +4524,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="10" t="s">
         <v>163</v>
       </c>
       <c r="B33" s="4">
@@ -4577,7 +4577,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="10" t="s">
         <v>168</v>
       </c>
       <c r="B34" s="4">
@@ -4630,7 +4630,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="10" t="s">
         <v>172</v>
       </c>
       <c r="B35" s="4">
@@ -4683,7 +4683,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="10" t="s">
         <v>176</v>
       </c>
       <c r="B36" s="4">
@@ -4736,7 +4736,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="10" t="s">
         <v>182</v>
       </c>
       <c r="B37" s="4">
@@ -4789,7 +4789,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="10">
         <v>42238835</v>
       </c>
       <c r="B38" s="4">
@@ -4842,7 +4842,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="10">
         <v>42226153</v>
       </c>
       <c r="B39" s="4">
@@ -4895,7 +4895,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="10">
         <v>42247976</v>
       </c>
       <c r="B40" s="4">
@@ -4948,7 +4948,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="10" t="s">
         <v>196</v>
       </c>
       <c r="B41" s="4">
@@ -5001,7 +5001,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="10">
         <v>42233189</v>
       </c>
       <c r="B42" s="4">
@@ -5054,7 +5054,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="10" t="s">
         <v>204</v>
       </c>
       <c r="B43" s="4">
@@ -5107,7 +5107,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="10" t="s">
         <v>207</v>
       </c>
       <c r="B44" s="4">
@@ -5160,7 +5160,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="10" t="s">
         <v>211</v>
       </c>
       <c r="B45" s="4">
@@ -5213,7 +5213,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="10" t="s">
         <v>215</v>
       </c>
       <c r="B46" s="4">
@@ -5266,7 +5266,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="10" t="s">
         <v>218</v>
       </c>
       <c r="B47" s="4">

</xml_diff>